<commit_message>
Screenshot for passed and Failed Test
</commit_message>
<xml_diff>
--- a/Output_ExcelSheet/Hospital.xlsx
+++ b/Output_ExcelSheet/Hospital.xlsx
@@ -41,10 +41,10 @@
     <t>Apollo First Med Hospitals</t>
   </si>
   <si>
-    <t>Eswar Medical Foundation</t>
+    <t>VS Hospitals</t>
   </si>
   <si>
-    <t>VS Hospitals</t>
+    <t>Jayam Hospital &amp; GFC Fertility</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Log file and multiple browsing feature added
</commit_message>
<xml_diff>
--- a/Output_ExcelSheet/Hospital.xlsx
+++ b/Output_ExcelSheet/Hospital.xlsx
@@ -41,10 +41,10 @@
     <t>Apollo First Med Hospitals</t>
   </si>
   <si>
-    <t>VS Hospitals</t>
+    <t>Jayam Hospital &amp; GFC Fertility</t>
   </si>
   <si>
-    <t>Jayam Hospital &amp; GFC Fertility</t>
+    <t>Maaya Speciality Hospitals</t>
   </si>
 </sst>
 </file>
@@ -89,13 +89,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="30.35546875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="30.3515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>